<commit_message>
TFT ET CPC a toute echelle
</commit_message>
<xml_diff>
--- a/module classe projet/ModulePrincipal/CPC.xlsx
+++ b/module classe projet/ModulePrincipal/CPC.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="CPC Mensuel" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CPC Trimestriel" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CPC Semestriel" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CPC Annuel" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>CPC Projet Ecole</t>
   </si>
@@ -68,9 +71,6 @@
     <t>Couts d'assurance</t>
   </si>
   <si>
-    <t>Cout mm</t>
-  </si>
-  <si>
     <t>TOTAL CHARGES D'EXPLOITATION</t>
   </si>
   <si>
@@ -102,6 +102,27 @@
   </si>
   <si>
     <t>RESULTAT NET</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>A1</t>
   </si>
 </sst>
 </file>
@@ -581,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,394 +782,1008 @@
         <v>16</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K10" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="E11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="G11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="H11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="I11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="J11" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="K11" s="6" t="n">
-        <v>200</v>
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="I12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="J12" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="K12" s="8" t="n">
-        <v>1200</v>
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="C13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="D13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="E13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="F13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="G13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="H13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="I13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="J13" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="K13" s="10" t="n">
-        <v>-1200</v>
+      <c r="B13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="3" t="n"/>
+      <c r="E14" s="3" t="n"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
+      <c r="H14" s="3" t="n"/>
+      <c r="I14" s="3" t="n"/>
+      <c r="J14" s="3" t="n"/>
+      <c r="K14" s="3" t="n"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="n"/>
-      <c r="C15" s="3" t="n"/>
-      <c r="D15" s="3" t="n"/>
-      <c r="E15" s="3" t="n"/>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
-      <c r="H15" s="3" t="n"/>
-      <c r="I15" s="3" t="n"/>
-      <c r="J15" s="3" t="n"/>
-      <c r="K15" s="3" t="n"/>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="10" t="n"/>
+      <c r="E16" s="10" t="n"/>
+      <c r="F16" s="10" t="n"/>
+      <c r="G16" s="10" t="n"/>
+      <c r="H16" s="10" t="n"/>
+      <c r="I16" s="10" t="n"/>
+      <c r="J16" s="10" t="n"/>
+      <c r="K16" s="10" t="n"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="10" t="n"/>
-      <c r="C17" s="10" t="n"/>
-      <c r="D17" s="10" t="n"/>
-      <c r="E17" s="10" t="n"/>
-      <c r="F17" s="10" t="n"/>
-      <c r="G17" s="10" t="n"/>
-      <c r="H17" s="10" t="n"/>
-      <c r="I17" s="10" t="n"/>
-      <c r="J17" s="10" t="n"/>
-      <c r="K17" s="10" t="n"/>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="3" t="n"/>
+      <c r="F17" s="3" t="n"/>
+      <c r="G17" s="3" t="n"/>
+      <c r="H17" s="3" t="n"/>
+      <c r="I17" s="3" t="n"/>
+      <c r="J17" s="3" t="n"/>
+      <c r="K17" s="3" t="n"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3" t="n"/>
-      <c r="C18" s="3" t="n"/>
-      <c r="D18" s="3" t="n"/>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
-      <c r="H18" s="3" t="n"/>
-      <c r="I18" s="3" t="n"/>
-      <c r="J18" s="3" t="n"/>
-      <c r="K18" s="3" t="n"/>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="6" t="n">
+      <c r="B19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="C20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="D20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="E20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="F20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="G20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="H20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="I20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="J20" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="K20" s="10" t="n">
-        <v>-1200</v>
+      <c r="B20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="11" t="n">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="9" t="s">
+      <c r="B21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="C22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="D22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="E22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="F22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="G22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="I22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="J22" s="10" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="K22" s="10" t="n">
-        <v>-1200</v>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="3" t="n"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="4" t="n"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="3" t="n"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="n"/>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="4" t="n"/>
+      <c r="E9" s="4" t="n"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="3" t="n"/>
+      <c r="E14" s="3" t="n"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="10" t="n"/>
+      <c r="E16" s="10" t="n"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="3" t="n"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="4" t="n"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="n"/>
+      <c r="C9" s="4" t="n"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="10" t="n"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="3" t="n"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="n"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="n"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="n"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="n"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="n"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="10" t="n"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="n"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>